<commit_message>
usando metrica de error absoluto medio
</commit_message>
<xml_diff>
--- a/predictions/global/AdaBoostRegressor/Comorbilidades.xlsx
+++ b/predictions/global/AdaBoostRegressor/Comorbilidades.xlsx
@@ -462,10 +462,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.5104980402060012</v>
+        <v>0.5141455444626758</v>
       </c>
       <c r="C2" t="n">
-        <v>0.9898348999150072</v>
+        <v>0.9897622703593392</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
@@ -480,10 +480,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.2385665528510029</v>
+        <v>0.2419097835045483</v>
       </c>
       <c r="C3" t="n">
-        <v>0.9953372107250285</v>
+        <v>0.995271867197829</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
@@ -498,10 +498,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.3702426277939377</v>
+        <v>0.338055960087607</v>
       </c>
       <c r="C4" t="n">
-        <v>0.9928773551281175</v>
+        <v>0.9934965550431772</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
@@ -516,10 +516,10 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.4154236759486921</v>
+        <v>0.4153349664147831</v>
       </c>
       <c r="C5" t="n">
-        <v>0.991808413876015</v>
+        <v>0.9918101631065696</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
@@ -534,10 +534,10 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.6555328321716093</v>
+        <v>0.7292360521529262</v>
       </c>
       <c r="C6" t="n">
-        <v>0.9807452835088004</v>
+        <v>0.9785804268676348</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
@@ -552,10 +552,10 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.3312468788026585</v>
+        <v>0.404058060215838</v>
       </c>
       <c r="C7" t="n">
-        <v>0.9954220784450948</v>
+        <v>0.9944158082032909</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
@@ -570,10 +570,10 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.1564064177872994</v>
+        <v>0.1526505001906213</v>
       </c>
       <c r="C8" t="n">
-        <v>0.9983879524018624</v>
+        <v>0.9984266638436701</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
@@ -588,10 +588,10 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.5518977647463018</v>
+        <v>0.5254954434052722</v>
       </c>
       <c r="C9" t="n">
-        <v>0.9967125024843823</v>
+        <v>0.9968697735794284</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
@@ -606,10 +606,10 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.1182236427116248</v>
+        <v>0.1045862308324393</v>
       </c>
       <c r="C10" t="n">
-        <v>0.9978403340255546</v>
+        <v>0.9980894572443918</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
@@ -624,10 +624,10 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.338282356258996</v>
+        <v>0.3012841367677325</v>
       </c>
       <c r="C11" t="n">
-        <v>0.9750064671661391</v>
+        <v>0.9777400304056636</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
@@ -642,10 +642,10 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.04953934404560188</v>
+        <v>0.04999187914524317</v>
       </c>
       <c r="C12" t="n">
-        <v>0.9985431324081562</v>
+        <v>0.9985298241229227</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
@@ -660,10 +660,10 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.08455869235847047</v>
+        <v>0.08414612021499523</v>
       </c>
       <c r="C13" t="n">
-        <v>0.9991979229081709</v>
+        <v>0.9992018363398451</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
@@ -678,10 +678,10 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.08750623379233541</v>
+        <v>0.08745618430458782</v>
       </c>
       <c r="C14" t="n">
-        <v>0.9988152196103363</v>
+        <v>0.9988158972495058</v>
       </c>
       <c r="D14" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Creado grafico de tipos de modelo
</commit_message>
<xml_diff>
--- a/predictions/global/AdaBoostRegressor/Comorbilidades.xlsx
+++ b/predictions/global/AdaBoostRegressor/Comorbilidades.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,6 +451,11 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
+          <t>MAE</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
           <t>Tipo</t>
         </is>
       </c>
@@ -462,12 +467,15 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.5141455444626758</v>
+        <v>0.4858260388868722</v>
       </c>
       <c r="C2" t="n">
-        <v>0.9897622703593392</v>
-      </c>
-      <c r="D2" t="inlineStr">
+        <v>0.9903261718552575</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0.5688422646190253</v>
+      </c>
+      <c r="E2" t="inlineStr">
         <is>
           <t>global</t>
         </is>
@@ -480,12 +488,15 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.2419097835045483</v>
+        <v>0.2357639951764815</v>
       </c>
       <c r="C3" t="n">
-        <v>0.995271867197829</v>
-      </c>
-      <c r="D3" t="inlineStr">
+        <v>0.995391986785256</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0.3843755001218409</v>
+      </c>
+      <c r="E3" t="inlineStr">
         <is>
           <t>global</t>
         </is>
@@ -498,12 +509,15 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.338055960087607</v>
+        <v>0.354228512740891</v>
       </c>
       <c r="C4" t="n">
-        <v>0.9934965550431772</v>
-      </c>
-      <c r="D4" t="inlineStr">
+        <v>0.9931854310920872</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0.4698397028756816</v>
+      </c>
+      <c r="E4" t="inlineStr">
         <is>
           <t>global</t>
         </is>
@@ -516,12 +530,15 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.4153349664147831</v>
+        <v>0.406772042895757</v>
       </c>
       <c r="C5" t="n">
-        <v>0.9918101631065696</v>
-      </c>
-      <c r="D5" t="inlineStr">
+        <v>0.9919790122346771</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.4952415476002354</v>
+      </c>
+      <c r="E5" t="inlineStr">
         <is>
           <t>global</t>
         </is>
@@ -534,12 +551,15 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.7292360521529262</v>
+        <v>0.7384315664895728</v>
       </c>
       <c r="C6" t="n">
-        <v>0.9785804268676348</v>
-      </c>
-      <c r="D6" t="inlineStr">
+        <v>0.9783103305233276</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.6639375116161906</v>
+      </c>
+      <c r="E6" t="inlineStr">
         <is>
           <t>global</t>
         </is>
@@ -552,12 +572,15 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.404058060215838</v>
+        <v>0.3631266388613507</v>
       </c>
       <c r="C7" t="n">
-        <v>0.9944158082032909</v>
-      </c>
-      <c r="D7" t="inlineStr">
+        <v>0.9949814915291805</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.4965276629928901</v>
+      </c>
+      <c r="E7" t="inlineStr">
         <is>
           <t>global</t>
         </is>
@@ -570,12 +593,15 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.1526505001906213</v>
+        <v>0.1556483113569549</v>
       </c>
       <c r="C8" t="n">
-        <v>0.9984266638436701</v>
-      </c>
-      <c r="D8" t="inlineStr">
+        <v>0.9983957660431915</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0.3309224161203504</v>
+      </c>
+      <c r="E8" t="inlineStr">
         <is>
           <t>global</t>
         </is>
@@ -588,12 +614,15 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.5254954434052722</v>
+        <v>0.4564187238483384</v>
       </c>
       <c r="C9" t="n">
-        <v>0.9968697735794284</v>
-      </c>
-      <c r="D9" t="inlineStr">
+        <v>0.9972812438886709</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.5581454810666486</v>
+      </c>
+      <c r="E9" t="inlineStr">
         <is>
           <t>global</t>
         </is>
@@ -606,12 +635,15 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.1045862308324393</v>
+        <v>0.1058018669828489</v>
       </c>
       <c r="C10" t="n">
-        <v>0.9980894572443918</v>
-      </c>
-      <c r="D10" t="inlineStr">
+        <v>0.9980672504508001</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0.2369360161650128</v>
+      </c>
+      <c r="E10" t="inlineStr">
         <is>
           <t>global</t>
         </is>
@@ -624,12 +656,15 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.3012841367677325</v>
+        <v>0.1986423075790961</v>
       </c>
       <c r="C11" t="n">
-        <v>0.9777400304056636</v>
-      </c>
-      <c r="D11" t="inlineStr">
+        <v>0.9853235826675191</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0.3425956061944328</v>
+      </c>
+      <c r="E11" t="inlineStr">
         <is>
           <t>global</t>
         </is>
@@ -642,12 +677,15 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.04999187914524317</v>
+        <v>0.05081863269278668</v>
       </c>
       <c r="C12" t="n">
-        <v>0.9985298241229227</v>
-      </c>
-      <c r="D12" t="inlineStr">
+        <v>0.9985055107115712</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0.1661962461621603</v>
+      </c>
+      <c r="E12" t="inlineStr">
         <is>
           <t>global</t>
         </is>
@@ -660,12 +698,15 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.08414612021499523</v>
+        <v>0.09974499197663596</v>
       </c>
       <c r="C13" t="n">
-        <v>0.9992018363398451</v>
-      </c>
-      <c r="D13" t="inlineStr">
+        <v>0.9990538740505828</v>
+      </c>
+      <c r="D13" t="n">
+        <v>0.2214877650927295</v>
+      </c>
+      <c r="E13" t="inlineStr">
         <is>
           <t>global</t>
         </is>
@@ -678,12 +719,15 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.08745618430458782</v>
+        <v>0.08996850467433244</v>
       </c>
       <c r="C14" t="n">
-        <v>0.9988158972495058</v>
-      </c>
-      <c r="D14" t="inlineStr">
+        <v>0.9987818819825056</v>
+      </c>
+      <c r="D14" t="n">
+        <v>0.2397878346241068</v>
+      </c>
+      <c r="E14" t="inlineStr">
         <is>
           <t>global</t>
         </is>

</xml_diff>

<commit_message>
Añadiendo nomnre de modelo
</commit_message>
<xml_diff>
--- a/predictions/global/AdaBoostRegressor/Comorbilidades.xlsx
+++ b/predictions/global/AdaBoostRegressor/Comorbilidades.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -459,6 +459,11 @@
           <t>Tipo</t>
         </is>
       </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Modelo</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -467,17 +472,31 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.4858260388868722</v>
+        <v>0.5039322783415993</v>
       </c>
       <c r="C2" t="n">
-        <v>0.9903261718552575</v>
+        <v>0.9899656381769188</v>
       </c>
       <c r="D2" t="n">
-        <v>0.5688422646190253</v>
+        <v>0.5815779036458114</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
           <t>global</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>MultiOutputRegressor(estimator=GridSearchCV(cv=5,
+                                            estimator=Pipeline(steps=[('model',
+                                                                       AdaBoostRegressor())]),
+                                            param_grid={'model__learning_rate': [0.1,
+                                                                                 0.5,
+                                                                                 1.0],
+                                                        'model__n_estimators': [50,
+                                                                                100,
+                                                                                150]},
+                                            scoring='neg_mean_squared_error'))</t>
         </is>
       </c>
     </row>
@@ -488,17 +507,31 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.2357639951764815</v>
+        <v>0.2393456043709881</v>
       </c>
       <c r="C3" t="n">
-        <v>0.995391986785256</v>
+        <v>0.9953219841434787</v>
       </c>
       <c r="D3" t="n">
-        <v>0.3843755001218409</v>
+        <v>0.3827753431510709</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
           <t>global</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>MultiOutputRegressor(estimator=GridSearchCV(cv=5,
+                                            estimator=Pipeline(steps=[('model',
+                                                                       AdaBoostRegressor())]),
+                                            param_grid={'model__learning_rate': [0.1,
+                                                                                 0.5,
+                                                                                 1.0],
+                                                        'model__n_estimators': [50,
+                                                                                100,
+                                                                                150]},
+                                            scoring='neg_mean_squared_error'))</t>
         </is>
       </c>
     </row>
@@ -509,17 +542,31 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.354228512740891</v>
+        <v>0.3381587479270987</v>
       </c>
       <c r="C4" t="n">
-        <v>0.9931854310920872</v>
+        <v>0.9934945776337086</v>
       </c>
       <c r="D4" t="n">
-        <v>0.4698397028756816</v>
+        <v>0.4628283649783701</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
           <t>global</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>MultiOutputRegressor(estimator=GridSearchCV(cv=5,
+                                            estimator=Pipeline(steps=[('model',
+                                                                       AdaBoostRegressor())]),
+                                            param_grid={'model__learning_rate': [0.1,
+                                                                                 0.5,
+                                                                                 1.0],
+                                                        'model__n_estimators': [50,
+                                                                                100,
+                                                                                150]},
+                                            scoring='neg_mean_squared_error'))</t>
         </is>
       </c>
     </row>
@@ -530,17 +577,31 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.406772042895757</v>
+        <v>0.3851566315294757</v>
       </c>
       <c r="C5" t="n">
-        <v>0.9919790122346771</v>
+        <v>0.9924052385526835</v>
       </c>
       <c r="D5" t="n">
-        <v>0.4952415476002354</v>
+        <v>0.4846726063545287</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
           <t>global</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>MultiOutputRegressor(estimator=GridSearchCV(cv=5,
+                                            estimator=Pipeline(steps=[('model',
+                                                                       AdaBoostRegressor())]),
+                                            param_grid={'model__learning_rate': [0.1,
+                                                                                 0.5,
+                                                                                 1.0],
+                                                        'model__n_estimators': [50,
+                                                                                100,
+                                                                                150]},
+                                            scoring='neg_mean_squared_error'))</t>
         </is>
       </c>
     </row>
@@ -551,17 +612,31 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.7384315664895728</v>
+        <v>0.6587938625413217</v>
       </c>
       <c r="C6" t="n">
-        <v>0.9783103305233276</v>
+        <v>0.9806494985043637</v>
       </c>
       <c r="D6" t="n">
-        <v>0.6639375116161906</v>
+        <v>0.6109652078713076</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
           <t>global</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>MultiOutputRegressor(estimator=GridSearchCV(cv=5,
+                                            estimator=Pipeline(steps=[('model',
+                                                                       AdaBoostRegressor())]),
+                                            param_grid={'model__learning_rate': [0.1,
+                                                                                 0.5,
+                                                                                 1.0],
+                                                        'model__n_estimators': [50,
+                                                                                100,
+                                                                                150]},
+                                            scoring='neg_mean_squared_error'))</t>
         </is>
       </c>
     </row>
@@ -572,17 +647,31 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.3631266388613507</v>
+        <v>0.2479756927424193</v>
       </c>
       <c r="C7" t="n">
-        <v>0.9949814915291805</v>
+        <v>0.9965729087833175</v>
       </c>
       <c r="D7" t="n">
-        <v>0.4965276629928901</v>
+        <v>0.3768828815660853</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
           <t>global</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>MultiOutputRegressor(estimator=GridSearchCV(cv=5,
+                                            estimator=Pipeline(steps=[('model',
+                                                                       AdaBoostRegressor())]),
+                                            param_grid={'model__learning_rate': [0.1,
+                                                                                 0.5,
+                                                                                 1.0],
+                                                        'model__n_estimators': [50,
+                                                                                100,
+                                                                                150]},
+                                            scoring='neg_mean_squared_error'))</t>
         </is>
       </c>
     </row>
@@ -593,17 +682,31 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.1556483113569549</v>
+        <v>0.1579536424331374</v>
       </c>
       <c r="C8" t="n">
-        <v>0.9983957660431915</v>
+        <v>0.9983720054873471</v>
       </c>
       <c r="D8" t="n">
-        <v>0.3309224161203504</v>
+        <v>0.3426586216972675</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
           <t>global</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>MultiOutputRegressor(estimator=GridSearchCV(cv=5,
+                                            estimator=Pipeline(steps=[('model',
+                                                                       AdaBoostRegressor())]),
+                                            param_grid={'model__learning_rate': [0.1,
+                                                                                 0.5,
+                                                                                 1.0],
+                                                        'model__n_estimators': [50,
+                                                                                100,
+                                                                                150]},
+                                            scoring='neg_mean_squared_error'))</t>
         </is>
       </c>
     </row>
@@ -614,17 +717,31 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.4564187238483384</v>
+        <v>0.5213271728323167</v>
       </c>
       <c r="C9" t="n">
-        <v>0.9972812438886709</v>
+        <v>0.9968946027779292</v>
       </c>
       <c r="D9" t="n">
-        <v>0.5581454810666486</v>
+        <v>0.5974129538515721</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
           <t>global</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>MultiOutputRegressor(estimator=GridSearchCV(cv=5,
+                                            estimator=Pipeline(steps=[('model',
+                                                                       AdaBoostRegressor())]),
+                                            param_grid={'model__learning_rate': [0.1,
+                                                                                 0.5,
+                                                                                 1.0],
+                                                        'model__n_estimators': [50,
+                                                                                100,
+                                                                                150]},
+                                            scoring='neg_mean_squared_error'))</t>
         </is>
       </c>
     </row>
@@ -635,17 +752,31 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.1058018669828489</v>
+        <v>0.1160246393334504</v>
       </c>
       <c r="C10" t="n">
-        <v>0.9980672504508001</v>
+        <v>0.9978805046095817</v>
       </c>
       <c r="D10" t="n">
-        <v>0.2369360161650128</v>
+        <v>0.2450065170048785</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
           <t>global</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>MultiOutputRegressor(estimator=GridSearchCV(cv=5,
+                                            estimator=Pipeline(steps=[('model',
+                                                                       AdaBoostRegressor())]),
+                                            param_grid={'model__learning_rate': [0.1,
+                                                                                 0.5,
+                                                                                 1.0],
+                                                        'model__n_estimators': [50,
+                                                                                100,
+                                                                                150]},
+                                            scoring='neg_mean_squared_error'))</t>
         </is>
       </c>
     </row>
@@ -656,17 +787,31 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.1986423075790961</v>
+        <v>0.3228709807900418</v>
       </c>
       <c r="C11" t="n">
-        <v>0.9853235826675191</v>
+        <v>0.9761451157290082</v>
       </c>
       <c r="D11" t="n">
-        <v>0.3425956061944328</v>
+        <v>0.4408833004892758</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
           <t>global</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>MultiOutputRegressor(estimator=GridSearchCV(cv=5,
+                                            estimator=Pipeline(steps=[('model',
+                                                                       AdaBoostRegressor())]),
+                                            param_grid={'model__learning_rate': [0.1,
+                                                                                 0.5,
+                                                                                 1.0],
+                                                        'model__n_estimators': [50,
+                                                                                100,
+                                                                                150]},
+                                            scoring='neg_mean_squared_error'))</t>
         </is>
       </c>
     </row>
@@ -677,17 +822,31 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.05081863269278668</v>
+        <v>0.04970959672068318</v>
       </c>
       <c r="C12" t="n">
-        <v>0.9985055107115712</v>
+        <v>0.9985381255674414</v>
       </c>
       <c r="D12" t="n">
-        <v>0.1661962461621603</v>
+        <v>0.1641097888004932</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
           <t>global</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>MultiOutputRegressor(estimator=GridSearchCV(cv=5,
+                                            estimator=Pipeline(steps=[('model',
+                                                                       AdaBoostRegressor())]),
+                                            param_grid={'model__learning_rate': [0.1,
+                                                                                 0.5,
+                                                                                 1.0],
+                                                        'model__n_estimators': [50,
+                                                                                100,
+                                                                                150]},
+                                            scoring='neg_mean_squared_error'))</t>
         </is>
       </c>
     </row>
@@ -698,17 +857,31 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.09974499197663596</v>
+        <v>0.1019808664031013</v>
       </c>
       <c r="C13" t="n">
-        <v>0.9990538740505828</v>
+        <v>0.999032665779645</v>
       </c>
       <c r="D13" t="n">
-        <v>0.2214877650927295</v>
+        <v>0.223878916912976</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
           <t>global</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>MultiOutputRegressor(estimator=GridSearchCV(cv=5,
+                                            estimator=Pipeline(steps=[('model',
+                                                                       AdaBoostRegressor())]),
+                                            param_grid={'model__learning_rate': [0.1,
+                                                                                 0.5,
+                                                                                 1.0],
+                                                        'model__n_estimators': [50,
+                                                                                100,
+                                                                                150]},
+                                            scoring='neg_mean_squared_error'))</t>
         </is>
       </c>
     </row>
@@ -719,17 +892,31 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.08996850467433244</v>
+        <v>0.09462228383192978</v>
       </c>
       <c r="C14" t="n">
-        <v>0.9987818819825056</v>
+        <v>0.9987188726853985</v>
       </c>
       <c r="D14" t="n">
-        <v>0.2397878346241068</v>
+        <v>0.2492067260330941</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
           <t>global</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>MultiOutputRegressor(estimator=GridSearchCV(cv=5,
+                                            estimator=Pipeline(steps=[('model',
+                                                                       AdaBoostRegressor())]),
+                                            param_grid={'model__learning_rate': [0.1,
+                                                                                 0.5,
+                                                                                 1.0],
+                                                        'model__n_estimators': [50,
+                                                                                100,
+                                                                                150]},
+                                            scoring='neg_mean_squared_error'))</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
elapsed time y cpu
</commit_message>
<xml_diff>
--- a/predictions/global/AdaBoostRegressor/Comorbilidades.xlsx
+++ b/predictions/global/AdaBoostRegressor/Comorbilidades.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -464,6 +464,16 @@
           <t>Modelo</t>
         </is>
       </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Elapsed Time</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>CPU</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -472,13 +482,13 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.5039322783415993</v>
+        <v>0.4972636062298078</v>
       </c>
       <c r="C2" t="n">
-        <v>0.9899656381769188</v>
+        <v>0.9900984256003985</v>
       </c>
       <c r="D2" t="n">
-        <v>0.5815779036458114</v>
+        <v>0.5737939481677846</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -498,6 +508,12 @@
                                                                                 150]},
                                             scoring='neg_mean_squared_error'))</t>
         </is>
+      </c>
+      <c r="G2" t="n">
+        <v>1.669922641383406</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0.97</v>
       </c>
     </row>
     <row r="3">
@@ -507,13 +523,13 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.2393456043709881</v>
+        <v>0.2376395757976146</v>
       </c>
       <c r="C3" t="n">
-        <v>0.9953219841434787</v>
+        <v>0.9953553285148486</v>
       </c>
       <c r="D3" t="n">
-        <v>0.3827753431510709</v>
+        <v>0.3829637447440828</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
@@ -533,6 +549,12 @@
                                                                                 150]},
                                             scoring='neg_mean_squared_error'))</t>
         </is>
+      </c>
+      <c r="G3" t="n">
+        <v>1.669922641383406</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0.97</v>
       </c>
     </row>
     <row r="4">
@@ -542,13 +564,13 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.3381587479270987</v>
+        <v>0.3440597266435089</v>
       </c>
       <c r="C4" t="n">
-        <v>0.9934945776337086</v>
+        <v>0.9933810559248661</v>
       </c>
       <c r="D4" t="n">
-        <v>0.4628283649783701</v>
+        <v>0.4635476650442505</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
@@ -568,6 +590,12 @@
                                                                                 150]},
                                             scoring='neg_mean_squared_error'))</t>
         </is>
+      </c>
+      <c r="G4" t="n">
+        <v>1.669922641383406</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0.97</v>
       </c>
     </row>
     <row r="5">
@@ -577,13 +605,13 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.3851566315294757</v>
+        <v>0.4134410054541373</v>
       </c>
       <c r="C5" t="n">
-        <v>0.9924052385526835</v>
+        <v>0.9918475094236497</v>
       </c>
       <c r="D5" t="n">
-        <v>0.4846726063545287</v>
+        <v>0.5003202100897108</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
@@ -603,6 +631,12 @@
                                                                                 150]},
                                             scoring='neg_mean_squared_error'))</t>
         </is>
+      </c>
+      <c r="G5" t="n">
+        <v>1.669922641383406</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0.97</v>
       </c>
     </row>
     <row r="6">
@@ -612,13 +646,13 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.6587938625413217</v>
+        <v>0.6666393828293923</v>
       </c>
       <c r="C6" t="n">
-        <v>0.9806494985043637</v>
+        <v>0.9804190550216592</v>
       </c>
       <c r="D6" t="n">
-        <v>0.6109652078713076</v>
+        <v>0.6111898016761881</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
@@ -638,6 +672,12 @@
                                                                                 150]},
                                             scoring='neg_mean_squared_error'))</t>
         </is>
+      </c>
+      <c r="G6" t="n">
+        <v>1.669922641383406</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0.97</v>
       </c>
     </row>
     <row r="7">
@@ -647,13 +687,13 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.2479756927424193</v>
+        <v>0.2476002055963841</v>
       </c>
       <c r="C7" t="n">
-        <v>0.9965729087833175</v>
+        <v>0.9965780981173442</v>
       </c>
       <c r="D7" t="n">
-        <v>0.3768828815660853</v>
+        <v>0.3764936609166029</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
@@ -673,6 +713,12 @@
                                                                                 150]},
                                             scoring='neg_mean_squared_error'))</t>
         </is>
+      </c>
+      <c r="G7" t="n">
+        <v>1.669922641383406</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0.97</v>
       </c>
     </row>
     <row r="8">
@@ -682,13 +728,13 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.1579536424331374</v>
+        <v>0.1533455515139108</v>
       </c>
       <c r="C8" t="n">
-        <v>0.9983720054873471</v>
+        <v>0.9984195000978843</v>
       </c>
       <c r="D8" t="n">
-        <v>0.3426586216972675</v>
+        <v>0.3352655043891136</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -708,6 +754,12 @@
                                                                                 150]},
                                             scoring='neg_mean_squared_error'))</t>
         </is>
+      </c>
+      <c r="G8" t="n">
+        <v>1.669922641383406</v>
+      </c>
+      <c r="H8" t="n">
+        <v>0.97</v>
       </c>
     </row>
     <row r="9">
@@ -717,13 +769,13 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.5213271728323167</v>
+        <v>0.4749149041100557</v>
       </c>
       <c r="C9" t="n">
-        <v>0.9968946027779292</v>
+        <v>0.9971710674202325</v>
       </c>
       <c r="D9" t="n">
-        <v>0.5974129538515721</v>
+        <v>0.5754557717508432</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
@@ -743,6 +795,12 @@
                                                                                 150]},
                                             scoring='neg_mean_squared_error'))</t>
         </is>
+      </c>
+      <c r="G9" t="n">
+        <v>1.669922641383406</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0.97</v>
       </c>
     </row>
     <row r="10">
@@ -752,13 +810,13 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.1160246393334504</v>
+        <v>0.1075861073149535</v>
       </c>
       <c r="C10" t="n">
-        <v>0.9978805046095817</v>
+        <v>0.9980346566053806</v>
       </c>
       <c r="D10" t="n">
-        <v>0.2450065170048785</v>
+        <v>0.2435166343840025</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
@@ -778,6 +836,12 @@
                                                                                 150]},
                                             scoring='neg_mean_squared_error'))</t>
         </is>
+      </c>
+      <c r="G10" t="n">
+        <v>1.669922641383406</v>
+      </c>
+      <c r="H10" t="n">
+        <v>0.97</v>
       </c>
     </row>
     <row r="11">
@@ -787,13 +851,13 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.3228709807900418</v>
+        <v>0.2540151239672845</v>
       </c>
       <c r="C11" t="n">
-        <v>0.9761451157290082</v>
+        <v>0.9812324372710919</v>
       </c>
       <c r="D11" t="n">
-        <v>0.4408833004892758</v>
+        <v>0.3884996060380089</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
@@ -813,6 +877,12 @@
                                                                                 150]},
                                             scoring='neg_mean_squared_error'))</t>
         </is>
+      </c>
+      <c r="G11" t="n">
+        <v>1.669922641383406</v>
+      </c>
+      <c r="H11" t="n">
+        <v>0.97</v>
       </c>
     </row>
     <row r="12">
@@ -822,13 +892,13 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.04970959672068318</v>
+        <v>0.05043507891103303</v>
       </c>
       <c r="C12" t="n">
-        <v>0.9985381255674414</v>
+        <v>0.9985167903739312</v>
       </c>
       <c r="D12" t="n">
-        <v>0.1641097888004932</v>
+        <v>0.1647042703662659</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
@@ -848,6 +918,12 @@
                                                                                 150]},
                                             scoring='neg_mean_squared_error'))</t>
         </is>
+      </c>
+      <c r="G12" t="n">
+        <v>1.669922641383406</v>
+      </c>
+      <c r="H12" t="n">
+        <v>0.97</v>
       </c>
     </row>
     <row r="13">
@@ -857,13 +933,13 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.1019808664031013</v>
+        <v>0.09783325630578199</v>
       </c>
       <c r="C13" t="n">
-        <v>0.999032665779645</v>
+        <v>0.9990720077201612</v>
       </c>
       <c r="D13" t="n">
-        <v>0.223878916912976</v>
+        <v>0.2199165099218983</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
@@ -883,6 +959,12 @@
                                                                                 150]},
                                             scoring='neg_mean_squared_error'))</t>
         </is>
+      </c>
+      <c r="G13" t="n">
+        <v>1.669922641383406</v>
+      </c>
+      <c r="H13" t="n">
+        <v>0.97</v>
       </c>
     </row>
     <row r="14">
@@ -892,13 +974,13 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.09462228383192978</v>
+        <v>0.08744915486079569</v>
       </c>
       <c r="C14" t="n">
-        <v>0.9987188726853985</v>
+        <v>0.9988159924238357</v>
       </c>
       <c r="D14" t="n">
-        <v>0.2492067260330941</v>
+        <v>0.2401551473425225</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
@@ -918,6 +1000,12 @@
                                                                                 150]},
                                             scoring='neg_mean_squared_error'))</t>
         </is>
+      </c>
+      <c r="G14" t="n">
+        <v>1.669922641383406</v>
+      </c>
+      <c r="H14" t="n">
+        <v>0.97</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Creado makefile con linter
</commit_message>
<xml_diff>
--- a/predictions/global/AdaBoostRegressor/Comorbilidades.xlsx
+++ b/predictions/global/AdaBoostRegressor/Comorbilidades.xlsx
@@ -482,13 +482,13 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.5045466359173274</v>
+        <v>0.4980883136293128</v>
       </c>
       <c r="C2" t="n">
-        <v>0.9899534050129233</v>
+        <v>0.9900820039247082</v>
       </c>
       <c r="D2" t="n">
-        <v>0.5769714387676189</v>
+        <v>0.5772119266417263</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -510,10 +510,10 @@
         </is>
       </c>
       <c r="G2" t="n">
-        <v>1.659619214700069</v>
+        <v>1.558460351833249</v>
       </c>
       <c r="H2" t="n">
-        <v>0.9740000000000001</v>
+        <v>0.9990000000000001</v>
       </c>
     </row>
     <row r="3">
@@ -523,13 +523,13 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.2402783075963036</v>
+        <v>0.239056291290989</v>
       </c>
       <c r="C3" t="n">
-        <v>0.9953037544354841</v>
+        <v>0.9953276387749029</v>
       </c>
       <c r="D3" t="n">
-        <v>0.3874686931750853</v>
+        <v>0.3843433050552175</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
@@ -551,10 +551,10 @@
         </is>
       </c>
       <c r="G3" t="n">
-        <v>1.659619214700069</v>
+        <v>1.558460351833249</v>
       </c>
       <c r="H3" t="n">
-        <v>0.9740000000000001</v>
+        <v>0.9990000000000001</v>
       </c>
     </row>
     <row r="4">
@@ -564,13 +564,13 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.3454596881162179</v>
+        <v>0.3424301550227666</v>
       </c>
       <c r="C4" t="n">
-        <v>0.9933541237791437</v>
+        <v>0.9934124052592661</v>
       </c>
       <c r="D4" t="n">
-        <v>0.472455093042543</v>
+        <v>0.4655874903828661</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
@@ -592,10 +592,10 @@
         </is>
       </c>
       <c r="G4" t="n">
-        <v>1.659619214700069</v>
+        <v>1.558460351833249</v>
       </c>
       <c r="H4" t="n">
-        <v>0.9740000000000001</v>
+        <v>0.9990000000000001</v>
       </c>
     </row>
     <row r="5">
@@ -605,13 +605,13 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.4128599214119167</v>
+        <v>0.4178647680449223</v>
       </c>
       <c r="C5" t="n">
-        <v>0.9918589676053873</v>
+        <v>0.9917602788820304</v>
       </c>
       <c r="D5" t="n">
-        <v>0.499073510059206</v>
+        <v>0.5037273826483598</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
@@ -633,10 +633,10 @@
         </is>
       </c>
       <c r="G5" t="n">
-        <v>1.659619214700069</v>
+        <v>1.558460351833249</v>
       </c>
       <c r="H5" t="n">
-        <v>0.9740000000000001</v>
+        <v>0.9990000000000001</v>
       </c>
     </row>
     <row r="6">
@@ -646,13 +646,13 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.7394283167332049</v>
+        <v>0.7195241642125411</v>
       </c>
       <c r="C6" t="n">
-        <v>0.9782810533576209</v>
+        <v>0.9788656904573576</v>
       </c>
       <c r="D6" t="n">
-        <v>0.6606343910563642</v>
+        <v>0.6549930491151482</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
@@ -674,10 +674,10 @@
         </is>
       </c>
       <c r="G6" t="n">
-        <v>1.659619214700069</v>
+        <v>1.558460351833249</v>
       </c>
       <c r="H6" t="n">
-        <v>0.9740000000000001</v>
+        <v>0.9990000000000001</v>
       </c>
     </row>
     <row r="7">
@@ -687,13 +687,13 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.3920953706048129</v>
+        <v>0.3829998621080163</v>
       </c>
       <c r="C7" t="n">
-        <v>0.9945811358127854</v>
+        <v>0.9947068382029508</v>
       </c>
       <c r="D7" t="n">
-        <v>0.5159153470454286</v>
+        <v>0.5150875870527777</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
@@ -715,10 +715,10 @@
         </is>
       </c>
       <c r="G7" t="n">
-        <v>1.659619214700069</v>
+        <v>1.558460351833249</v>
       </c>
       <c r="H7" t="n">
-        <v>0.9740000000000001</v>
+        <v>0.9990000000000001</v>
       </c>
     </row>
     <row r="8">
@@ -728,13 +728,13 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.1535922851531537</v>
+        <v>0.1529799275151037</v>
       </c>
       <c r="C8" t="n">
-        <v>0.9984169570668748</v>
+        <v>0.9984232685064792</v>
       </c>
       <c r="D8" t="n">
-        <v>0.3333723370868232</v>
+        <v>0.3311603784071903</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -756,10 +756,10 @@
         </is>
       </c>
       <c r="G8" t="n">
-        <v>1.659619214700069</v>
+        <v>1.558460351833249</v>
       </c>
       <c r="H8" t="n">
-        <v>0.9740000000000001</v>
+        <v>0.9990000000000001</v>
       </c>
     </row>
     <row r="9">
@@ -769,13 +769,13 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.572736473495928</v>
+        <v>0.4978591271369693</v>
       </c>
       <c r="C9" t="n">
-        <v>0.9965883722421179</v>
+        <v>0.9970343952301695</v>
       </c>
       <c r="D9" t="n">
-        <v>0.6267713950095176</v>
+        <v>0.5844367220048292</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
@@ -797,10 +797,10 @@
         </is>
       </c>
       <c r="G9" t="n">
-        <v>1.659619214700069</v>
+        <v>1.558460351833249</v>
       </c>
       <c r="H9" t="n">
-        <v>0.9740000000000001</v>
+        <v>0.9990000000000001</v>
       </c>
     </row>
     <row r="10">
@@ -810,13 +810,13 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.1059353069008138</v>
+        <v>0.1044224412242731</v>
       </c>
       <c r="C10" t="n">
-        <v>0.9980648128195121</v>
+        <v>0.9980924492926455</v>
       </c>
       <c r="D10" t="n">
-        <v>0.2365836036214232</v>
+        <v>0.2348577086854635</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
@@ -838,10 +838,10 @@
         </is>
       </c>
       <c r="G10" t="n">
-        <v>1.659619214700069</v>
+        <v>1.558460351833249</v>
       </c>
       <c r="H10" t="n">
-        <v>0.9740000000000001</v>
+        <v>0.9990000000000001</v>
       </c>
     </row>
     <row r="11">
@@ -851,13 +851,13 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.3462600922022194</v>
+        <v>0.3134948840143841</v>
       </c>
       <c r="C11" t="n">
-        <v>0.9744170429719782</v>
+        <v>0.97683785591566</v>
       </c>
       <c r="D11" t="n">
-        <v>0.4512428529696779</v>
+        <v>0.4293759673639526</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
@@ -879,10 +879,10 @@
         </is>
       </c>
       <c r="G11" t="n">
-        <v>1.659619214700069</v>
+        <v>1.558460351833249</v>
       </c>
       <c r="H11" t="n">
-        <v>0.9740000000000001</v>
+        <v>0.9990000000000001</v>
       </c>
     </row>
     <row r="12">
@@ -892,13 +892,13 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.04973323411665719</v>
+        <v>0.05243601867023975</v>
       </c>
       <c r="C12" t="n">
-        <v>0.9985374304319523</v>
+        <v>0.9984579461493137</v>
       </c>
       <c r="D12" t="n">
-        <v>0.1634941780466908</v>
+        <v>0.1633510054277421</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
@@ -920,10 +920,10 @@
         </is>
       </c>
       <c r="G12" t="n">
-        <v>1.659619214700069</v>
+        <v>1.558460351833249</v>
       </c>
       <c r="H12" t="n">
-        <v>0.9740000000000001</v>
+        <v>0.9990000000000001</v>
       </c>
     </row>
     <row r="13">
@@ -933,13 +933,13 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.07380766386120099</v>
+        <v>0.07632337034479625</v>
       </c>
       <c r="C13" t="n">
-        <v>0.9992999012315193</v>
+        <v>0.9992760386281136</v>
       </c>
       <c r="D13" t="n">
-        <v>0.2056211035010789</v>
+        <v>0.2081515299792747</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
@@ -961,10 +961,10 @@
         </is>
       </c>
       <c r="G13" t="n">
-        <v>1.659619214700069</v>
+        <v>1.558460351833249</v>
       </c>
       <c r="H13" t="n">
-        <v>0.9740000000000001</v>
+        <v>0.9990000000000001</v>
       </c>
     </row>
     <row r="14">
@@ -974,13 +974,13 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.08906863778579398</v>
+        <v>0.08726761627618847</v>
       </c>
       <c r="C14" t="n">
-        <v>0.9987940656247063</v>
+        <v>0.998818450344211</v>
       </c>
       <c r="D14" t="n">
-        <v>0.2407484512208981</v>
+        <v>0.2390931973700207</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
@@ -1002,10 +1002,10 @@
         </is>
       </c>
       <c r="G14" t="n">
-        <v>1.659619214700069</v>
+        <v>1.558460351833249</v>
       </c>
       <c r="H14" t="n">
-        <v>0.9740000000000001</v>
+        <v>0.9990000000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>